<commit_message>
update descripciones de datos
</commit_message>
<xml_diff>
--- a/data/diccionario de datos ingresos a juzg.xlsx
+++ b/data/diccionario de datos ingresos a juzg.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t xml:space="preserve">Variables </t>
   </si>
@@ -31,6 +31,9 @@
     <t>Clave única de identificación del expediente</t>
   </si>
   <si>
+    <t>con este número aparece en la consulta pública? seria ubicable: exp_cuij+exp_anio+exp_sufijo</t>
+  </si>
+  <si>
     <t>org_idintpri</t>
   </si>
   <si>
@@ -67,12 +70,18 @@
     <t>Código  numérico del estado del expediente</t>
   </si>
   <si>
+    <t xml:space="preserve">identificador unico que intanta estandarizar </t>
+  </si>
+  <si>
     <t>est_descr</t>
   </si>
   <si>
     <t>Descripción del estado del expediente</t>
   </si>
   <si>
+    <t>estado administrativo posibles = inicial archivado anulado (SABRI)  *no estan automatizados *dependen de la carga manual</t>
+  </si>
+  <si>
     <t>exp_anio</t>
   </si>
   <si>
@@ -97,6 +106,9 @@
     <t>Indica si en ese expediente hay detenidos  (0: NO/1: Sí)</t>
   </si>
   <si>
+    <t>en realidad indica si hubo al inicio del caso, no es la unica variable hay otras, por lo que el 0 no necesariamente indica que no pueda haber detenido en el expte (SABRI)</t>
+  </si>
+  <si>
     <t>exp_id</t>
   </si>
   <si>
@@ -109,6 +121,9 @@
     <t>Indica si el expediente es principal o incidente. (0:Principal  / &gt;=1:Incidente)</t>
   </si>
   <si>
+    <t>importante los 0 porque los &gt;1 los crea cada Juzgado de manera no normada</t>
+  </si>
+  <si>
     <t>exp_fechecho</t>
   </si>
   <si>
@@ -133,12 +148,18 @@
     <t>Fecha de registro en el juzgado</t>
   </si>
   <si>
+    <t>la diferencia entre esta fecha y la exp_fechecho</t>
+  </si>
+  <si>
     <t>exp_fecsor</t>
   </si>
   <si>
     <t xml:space="preserve">Fecha de sorteo del expediente </t>
   </si>
   <si>
+    <t xml:space="preserve">debería ser anterior a exp_fecreg </t>
+  </si>
+  <si>
     <t>exp_fecelev</t>
   </si>
   <si>
@@ -157,12 +178,18 @@
     <t>Código numérico del delito</t>
   </si>
   <si>
+    <t>la que sirve es oju_descr</t>
+  </si>
+  <si>
     <t>oju_descr</t>
   </si>
   <si>
     <t>Descripción del delito</t>
   </si>
   <si>
+    <t>existe diccionario? (SABRI)</t>
+  </si>
+  <si>
     <t>exp_ultmov</t>
   </si>
   <si>
@@ -193,6 +220,9 @@
     <t>Forma de ingreso del hecho</t>
   </si>
   <si>
+    <t>existe diccionario?</t>
+  </si>
+  <si>
     <t>org_cod</t>
   </si>
   <si>
@@ -278,6 +308,9 @@
   </si>
   <si>
     <t>den_fec_hecho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la diferencia con </t>
   </si>
   <si>
     <t>den_fec_ingreso_MPF</t>
@@ -432,11 +465,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -497,12 +535,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B64" displayName="Table_1" id="1">
-  <tableColumns count="2">
-    <tableColumn name="Variables " id="1"/>
-    <tableColumn name="Definición" id="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:C64" displayName="Table_1" id="1">
+  <tableColumns count="3">
+    <tableColumn name="Column1" id="1"/>
+    <tableColumn name="Column2" id="2"/>
+    <tableColumn name="Column3" id="3"/>
   </tableColumns>
   <tableStyleInfo name="Hoja1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
+    </ext>
+  </extLst>
 </table>
 </file>
 
@@ -712,7 +756,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="19.25"/>
     <col customWidth="1" min="2" max="2" width="76.75"/>
-    <col customWidth="1" min="3" max="26" width="9.38"/>
+    <col customWidth="1" min="3" max="3" width="124.5"/>
+    <col customWidth="1" min="4" max="26" width="9.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -722,6 +767,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -730,6 +776,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -738,1094 +785,1177 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>67</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>69</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>81</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>90</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>94</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="A49" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49" s="5"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="A50" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" s="5"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>100</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C51" s="2"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="C52" s="2"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C53" s="2"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="A54" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="5"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>106</v>
-      </c>
+      <c r="A55" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="5"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>109</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="C56" s="2"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>111</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="C57" s="2"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>113</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C58" s="2"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>115</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C59" s="2"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>117</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C60" s="2"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>119</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C61" s="2"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C62" s="2"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>123</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C63" s="2"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="C64" s="2"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="3"/>
+      <c r="A65" s="6"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="3"/>
+      <c r="A66" s="6"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="3"/>
+      <c r="A67" s="6"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="3"/>
+      <c r="A68" s="6"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="3"/>
+      <c r="A69" s="6"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="3"/>
+      <c r="A70" s="6"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="3"/>
+      <c r="A71" s="6"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="3"/>
+      <c r="A72" s="6"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="3"/>
+      <c r="A73" s="6"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="3"/>
+      <c r="A74" s="6"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="3"/>
+      <c r="A75" s="6"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="3"/>
+      <c r="A76" s="6"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="3"/>
+      <c r="A77" s="6"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="3"/>
+      <c r="A78" s="6"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="3"/>
+      <c r="A79" s="6"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="3"/>
+      <c r="A80" s="6"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="3"/>
+      <c r="A81" s="6"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="3"/>
+      <c r="A82" s="6"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="3"/>
+      <c r="A83" s="6"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="3"/>
+      <c r="A84" s="6"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="3"/>
+      <c r="A85" s="6"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="3"/>
+      <c r="A86" s="6"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="3"/>
+      <c r="A87" s="6"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="3"/>
+      <c r="A88" s="6"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="3"/>
+      <c r="A89" s="6"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="3"/>
+      <c r="A90" s="6"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="3"/>
+      <c r="A91" s="6"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="3"/>
+      <c r="A92" s="6"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="3"/>
+      <c r="A93" s="6"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="3"/>
+      <c r="A94" s="6"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="3"/>
+      <c r="A95" s="6"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="3"/>
+      <c r="A96" s="6"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="3"/>
+      <c r="A97" s="6"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="3"/>
+      <c r="A98" s="6"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="3"/>
+      <c r="A99" s="6"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="3"/>
+      <c r="A100" s="6"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="3"/>
+      <c r="A101" s="6"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="3"/>
+      <c r="A102" s="6"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="3"/>
+      <c r="A103" s="6"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="3"/>
+      <c r="A104" s="6"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="3"/>
+      <c r="A105" s="6"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="3"/>
+      <c r="A106" s="6"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="3"/>
+      <c r="A107" s="6"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="3"/>
+      <c r="A108" s="6"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="3"/>
+      <c r="A109" s="6"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="3"/>
+      <c r="A110" s="6"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="3"/>
+      <c r="A111" s="6"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="3"/>
+      <c r="A112" s="6"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="3"/>
+      <c r="A113" s="6"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="3"/>
+      <c r="A114" s="6"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="3"/>
+      <c r="A115" s="6"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="3"/>
+      <c r="A116" s="6"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="3"/>
+      <c r="A117" s="6"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="3"/>
+      <c r="A118" s="6"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="3"/>
+      <c r="A119" s="6"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="3"/>
+      <c r="A120" s="6"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="3"/>
+      <c r="A121" s="6"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="3"/>
+      <c r="A122" s="6"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="3"/>
+      <c r="A123" s="6"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="3"/>
+      <c r="A124" s="6"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="3"/>
+      <c r="A125" s="6"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="3"/>
+      <c r="A126" s="6"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="3"/>
+      <c r="A127" s="6"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="3"/>
+      <c r="A128" s="6"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="3"/>
+      <c r="A129" s="6"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="3"/>
+      <c r="A130" s="6"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="3"/>
+      <c r="A131" s="6"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="3"/>
+      <c r="A132" s="6"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="3"/>
+      <c r="A133" s="6"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="3"/>
+      <c r="A134" s="6"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="3"/>
+      <c r="A135" s="6"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="3"/>
+      <c r="A136" s="6"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="3"/>
+      <c r="A137" s="6"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="3"/>
+      <c r="A138" s="6"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="3"/>
+      <c r="A139" s="6"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="3"/>
+      <c r="A140" s="6"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="3"/>
+      <c r="A141" s="6"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="3"/>
+      <c r="A142" s="6"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="3"/>
+      <c r="A143" s="6"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="3"/>
+      <c r="A144" s="6"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="3"/>
+      <c r="A145" s="6"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="3"/>
+      <c r="A146" s="6"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="3"/>
+      <c r="A147" s="6"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="3"/>
+      <c r="A148" s="6"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="3"/>
+      <c r="A149" s="6"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="3"/>
+      <c r="A150" s="6"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="3"/>
+      <c r="A151" s="6"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="3"/>
+      <c r="A152" s="6"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="3"/>
+      <c r="A153" s="6"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="3"/>
+      <c r="A154" s="6"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="3"/>
+      <c r="A155" s="6"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="3"/>
+      <c r="A156" s="6"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="3"/>
+      <c r="A157" s="6"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="3"/>
+      <c r="A158" s="6"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="3"/>
+      <c r="A159" s="6"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="3"/>
+      <c r="A160" s="6"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="3"/>
+      <c r="A161" s="6"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="3"/>
+      <c r="A162" s="6"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="3"/>
+      <c r="A163" s="6"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="3"/>
+      <c r="A164" s="6"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="3"/>
+      <c r="A165" s="6"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="3"/>
+      <c r="A166" s="6"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="3"/>
+      <c r="A167" s="6"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="3"/>
+      <c r="A168" s="6"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="3"/>
+      <c r="A169" s="6"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="3"/>
+      <c r="A170" s="6"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="3"/>
+      <c r="A171" s="6"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="3"/>
+      <c r="A172" s="6"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="3"/>
+      <c r="A173" s="6"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="3"/>
+      <c r="A174" s="6"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="3"/>
+      <c r="A175" s="6"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="3"/>
+      <c r="A176" s="6"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="3"/>
+      <c r="A177" s="6"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="3"/>
+      <c r="A178" s="6"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="3"/>
+      <c r="A179" s="6"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="3"/>
+      <c r="A180" s="6"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="3"/>
+      <c r="A181" s="6"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="3"/>
+      <c r="A182" s="6"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="3"/>
+      <c r="A183" s="6"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="3"/>
+      <c r="A184" s="6"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="3"/>
+      <c r="A185" s="6"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="3"/>
+      <c r="A186" s="6"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="3"/>
+      <c r="A187" s="6"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="3"/>
+      <c r="A188" s="6"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="3"/>
+      <c r="A189" s="6"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="3"/>
+      <c r="A190" s="6"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="3"/>
+      <c r="A191" s="6"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="3"/>
+      <c r="A192" s="6"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="3"/>
+      <c r="A193" s="6"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="3"/>
+      <c r="A194" s="6"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="3"/>
+      <c r="A195" s="6"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="3"/>
+      <c r="A196" s="6"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="3"/>
+      <c r="A197" s="6"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="3"/>
+      <c r="A198" s="6"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="3"/>
+      <c r="A199" s="6"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="3"/>
+      <c r="A200" s="6"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="3"/>
+      <c r="A201" s="6"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="3"/>
+      <c r="A202" s="6"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="3"/>
+      <c r="A203" s="6"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="3"/>
+      <c r="A204" s="6"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="3"/>
+      <c r="A205" s="6"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="3"/>
+      <c r="A206" s="6"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="3"/>
+      <c r="A207" s="6"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="3"/>
+      <c r="A208" s="6"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="3"/>
+      <c r="A209" s="6"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="3"/>
+      <c r="A210" s="6"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="3"/>
+      <c r="A211" s="6"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="3"/>
+      <c r="A212" s="6"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="3"/>
+      <c r="A213" s="6"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="3"/>
+      <c r="A214" s="6"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="3"/>
+      <c r="A215" s="6"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="3"/>
+      <c r="A216" s="6"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="3"/>
+      <c r="A217" s="6"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="3"/>
+      <c r="A218" s="6"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="3"/>
+      <c r="A219" s="6"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="3"/>
+      <c r="A220" s="6"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="3"/>
+      <c r="A221" s="6"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="3"/>
+      <c r="A222" s="6"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="A223" s="3"/>
+      <c r="A223" s="6"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="A224" s="3"/>
+      <c r="A224" s="6"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="A225" s="3"/>
+      <c r="A225" s="6"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="A226" s="3"/>
+      <c r="A226" s="6"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="A227" s="3"/>
+      <c r="A227" s="6"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="A228" s="3"/>
+      <c r="A228" s="6"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="A229" s="3"/>
+      <c r="A229" s="6"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="A230" s="3"/>
+      <c r="A230" s="6"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="A231" s="3"/>
+      <c r="A231" s="6"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="3"/>
+      <c r="A232" s="6"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="A233" s="3"/>
+      <c r="A233" s="6"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="A234" s="3"/>
+      <c r="A234" s="6"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="A235" s="3"/>
+      <c r="A235" s="6"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="3"/>
+      <c r="A236" s="6"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="3"/>
+      <c r="A237" s="6"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="A238" s="3"/>
+      <c r="A238" s="6"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="A239" s="3"/>
+      <c r="A239" s="6"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="A240" s="3"/>
+      <c r="A240" s="6"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="A241" s="3"/>
+      <c r="A241" s="6"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="A242" s="3"/>
+      <c r="A242" s="6"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="A243" s="3"/>
+      <c r="A243" s="6"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="A244" s="3"/>
+      <c r="A244" s="6"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="A245" s="3"/>
+      <c r="A245" s="6"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="A246" s="3"/>
+      <c r="A246" s="6"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="A247" s="3"/>
+      <c r="A247" s="6"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="A248" s="3"/>
+      <c r="A248" s="6"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="3"/>
+      <c r="A249" s="6"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="3"/>
+      <c r="A250" s="6"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="A251" s="3"/>
+      <c r="A251" s="6"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="A252" s="3"/>
+      <c r="A252" s="6"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="A253" s="3"/>
+      <c r="A253" s="6"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="A254" s="3"/>
+      <c r="A254" s="6"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="A255" s="3"/>
+      <c r="A255" s="6"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="A256" s="3"/>
+      <c r="A256" s="6"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="A257" s="3"/>
+      <c r="A257" s="6"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="A258" s="3"/>
+      <c r="A258" s="6"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="A259" s="3"/>
+      <c r="A259" s="6"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="A260" s="3"/>
+      <c r="A260" s="6"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="A261" s="3"/>
+      <c r="A261" s="6"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="A262" s="3"/>
+      <c r="A262" s="6"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="A263" s="3"/>
+      <c r="A263" s="6"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="A264" s="3"/>
+      <c r="A264" s="6"/>
     </row>
     <row r="265" ht="15.75" customHeight="1"/>
     <row r="266" ht="15.75" customHeight="1"/>

</xml_diff>